<commit_message>
Atualização automática da planilha
</commit_message>
<xml_diff>
--- a/template-softexpert.xlsx
+++ b/template-softexpert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://planoeplano-my.sharepoint.com/personal/lucas_fernandes_planoeplano_com_br/Documents/Área de Trabalho/Softexpert/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_DDF5B26E4F51C3A50BC009EB0FEE48632AD81A56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A43420B-8CF9-4615-88B3-256387CA71D3}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_DDF5B26E4F51C3A50BC009EB0FEE48632AD81A56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98C2192F-B18E-4994-B149-43C8A8E66F20}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -726,7 +726,7 @@
     <t>Sponsor Executivo</t>
   </si>
   <si>
-    <t>Lucas Fern</t>
+    <t>Luciano</t>
   </si>
   <si>
     <t>VP Operações</t>
@@ -3806,7 +3806,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O17" sqref="O17"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.45"/>
@@ -4988,26 +4988,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="25b7c34c-a120-4ac3-ab60-c6bebc005a32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2aea894b-94ad-406a-ad4e-500caf6a56d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007CE54C9533A3014183E6B22E76F8A7A8" ma:contentTypeVersion="11" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="62704d92a99242f62405766f37cfe174">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="25b7c34c-a120-4ac3-ab60-c6bebc005a32" xmlns:ns3="2aea894b-94ad-406a-ad4e-500caf6a56d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e1ec24d789b63e7aafd81facc8b57960" ns2:_="" ns3:_="">
     <xsd:import namespace="25b7c34c-a120-4ac3-ab60-c6bebc005a32"/>
@@ -5202,8 +5182,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="25b7c34c-a120-4ac3-ab60-c6bebc005a32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2aea894b-94ad-406a-ad4e-500caf6a56d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DEC2584-7248-478C-8D26-41D0EBEC5C0F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B74F61-742C-4C28-9986-EBE675E88F9C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5211,5 +5211,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B74F61-742C-4C28-9986-EBE675E88F9C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DEC2584-7248-478C-8D26-41D0EBEC5C0F}"/>
 </file>
</xml_diff>